<commit_message>
Arquivos de entrada atualizados
</commit_message>
<xml_diff>
--- a/Código/VRQ - poços.xlsx
+++ b/Código/VRQ - poços.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thainá\Dropbox\Disciplinas\8° período\Introdução à Ciência de Dados\Atividades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thainá\Dropbox\Disciplinas\8° período\Introdução à Ciência de Dados\meu\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -98,9 +98,6 @@
     <t>Cor</t>
   </si>
   <si>
-    <t>Turb</t>
-  </si>
-  <si>
     <t>Coliformes totais</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>E. Coli</t>
+  </si>
+  <si>
+    <t>Turbidez</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,22 +507,22 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>